<commit_message>
Convert XML to JSON
</commit_message>
<xml_diff>
--- a/Doc/Phase1_Plan.xlsx
+++ b/Doc/Phase1_Plan.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thach\Workspace\Indv\imitori\Plan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27022"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="24255" windowHeight="12975"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="24260" windowHeight="19260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Develop Step" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Phase1 GOAL</t>
   </si>
@@ -129,13 +128,67 @@
   </si>
   <si>
     <t>9月</t>
+  </si>
+  <si>
+    <t>Bước 1</t>
+  </si>
+  <si>
+    <t>Tra được nghĩa của từ</t>
+  </si>
+  <si>
+    <t>Tra được mẫu câu ví dụ</t>
+  </si>
+  <si>
+    <t>Bước 2</t>
+  </si>
+  <si>
+    <t>Tra được từ liên quan</t>
+  </si>
+  <si>
+    <t>Thêm thông tin từ loại của từ</t>
+  </si>
+  <si>
+    <t>Phân tích Kanji</t>
+  </si>
+  <si>
+    <t>Bước 3</t>
+  </si>
+  <si>
+    <t>Tra nghĩa cho từ kèm theo câu ví dụ</t>
+  </si>
+  <si>
+    <t>Thêm thông tin độ khó cho từ</t>
+  </si>
+  <si>
+    <t>Bước 4</t>
+  </si>
+  <si>
+    <t>Thêm hình ảnh cho mỗi từ</t>
+  </si>
+  <si>
+    <t>Ảnh có nội dung liên quan đến từ (lấy trong mina, somatome..)</t>
+  </si>
+  <si>
+    <t>Bước 5</t>
+  </si>
+  <si>
+    <t>Tạo Flashcard</t>
+  </si>
+  <si>
+    <t>Bước 6</t>
+  </si>
+  <si>
+    <t>Tạo Quiz</t>
+  </si>
+  <si>
+    <t>Tạo Dokkai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,80 +249,80 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -278,184 +331,184 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="dotted">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,15 +533,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -530,9 +574,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -567,7 +620,7 @@
         <xdr:cNvPr id="9" name="グループ化 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD9F3E44-F80A-4625-A7E6-BAE1F68475E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD9F3E44-F80A-4625-A7E6-BAE1F68475E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -575,8 +628,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7553325" y="11972925"/>
-          <a:ext cx="1103444" cy="485775"/>
+          <a:off x="8566150" y="11430000"/>
+          <a:ext cx="1243144" cy="485775"/>
           <a:chOff x="7553325" y="9048750"/>
           <a:chExt cx="1103444" cy="502685"/>
         </a:xfrm>
@@ -593,7 +646,7 @@
           <xdr:cNvPr id="7" name="二等辺三角形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A44AAAB-DC3B-45D5-9DD4-EF7C0C9F4E86}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A44AAAB-DC3B-45D5-9DD4-EF7C0C9F4E86}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -638,7 +691,7 @@
           <xdr:cNvPr id="8" name="テキスト ボックス 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E2E605-F054-413E-AE7B-353609FE0A47}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15E2E605-F054-413E-AE7B-353609FE0A47}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -708,7 +761,7 @@
         <xdr:cNvPr id="10" name="グループ化 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE06C266-6BB4-4F4B-975B-FE417176C85B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE06C266-6BB4-4F4B-975B-FE417176C85B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -716,8 +769,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7029450" y="11220455"/>
-          <a:ext cx="1097352" cy="436018"/>
+          <a:off x="7972425" y="10687055"/>
+          <a:ext cx="1237052" cy="436018"/>
           <a:chOff x="7553325" y="9048750"/>
           <a:chExt cx="1097352" cy="605552"/>
         </a:xfrm>
@@ -734,7 +787,7 @@
           <xdr:cNvPr id="11" name="二等辺三角形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E18DA01-7038-4A9D-8238-75D988FC420F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E18DA01-7038-4A9D-8238-75D988FC420F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -779,7 +832,7 @@
           <xdr:cNvPr id="12" name="テキスト ボックス 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23319F69-28AD-4AC1-A031-BB0F17676040}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23319F69-28AD-4AC1-A031-BB0F17676040}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -844,7 +897,7 @@
         <xdr:cNvPr id="13" name="グループ化 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C55BC543-28AC-4966-81A0-D95F2EA8BDD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C55BC543-28AC-4966-81A0-D95F2EA8BDD4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -852,8 +905,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6877050" y="7639055"/>
-          <a:ext cx="1358449" cy="436018"/>
+          <a:off x="7785100" y="7153280"/>
+          <a:ext cx="1567999" cy="436018"/>
           <a:chOff x="7410450" y="9048750"/>
           <a:chExt cx="1358449" cy="605552"/>
         </a:xfrm>
@@ -870,7 +923,7 @@
           <xdr:cNvPr id="14" name="二等辺三角形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD66D61C-951B-486B-B8B3-43A7AFF4E807}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD66D61C-951B-486B-B8B3-43A7AFF4E807}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -915,7 +968,7 @@
           <xdr:cNvPr id="15" name="テキスト ボックス 14">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B646549B-83AF-4C4A-8C02-0E5508BF8521}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B646549B-83AF-4C4A-8C02-0E5508BF8521}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -985,7 +1038,7 @@
         <xdr:cNvPr id="16" name="グループ化 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E83283F3-0D5D-4723-9A4F-2AC6489F8B7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E83283F3-0D5D-4723-9A4F-2AC6489F8B7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -993,8 +1046,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2667000" y="8420105"/>
-          <a:ext cx="1011495" cy="436018"/>
+          <a:off x="3016250" y="7924805"/>
+          <a:ext cx="1151195" cy="436018"/>
           <a:chOff x="7562850" y="9048750"/>
           <a:chExt cx="1011495" cy="605552"/>
         </a:xfrm>
@@ -1011,7 +1064,7 @@
           <xdr:cNvPr id="17" name="二等辺三角形 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F319F1F-3200-4475-AE78-FD8B2A656CAF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F319F1F-3200-4475-AE78-FD8B2A656CAF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1056,7 +1109,7 @@
           <xdr:cNvPr id="18" name="テキスト ボックス 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B325C73-C2FB-4F70-924B-9EB68FD6F71A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1B325C73-C2FB-4F70-924B-9EB68FD6F71A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1126,7 +1179,7 @@
         <xdr:cNvPr id="19" name="グループ化 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{540E4344-96DF-45B0-A607-2B01009330D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{540E4344-96DF-45B0-A607-2B01009330D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1134,8 +1187,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4276725" y="9172580"/>
-          <a:ext cx="1423210" cy="436018"/>
+          <a:off x="4835525" y="8667755"/>
+          <a:ext cx="1632760" cy="436018"/>
           <a:chOff x="7381875" y="9048750"/>
           <a:chExt cx="1423210" cy="605552"/>
         </a:xfrm>
@@ -1152,7 +1205,7 @@
           <xdr:cNvPr id="20" name="二等辺三角形 19">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48441E5F-02DE-46E4-96C2-A9B1B0111609}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48441E5F-02DE-46E4-96C2-A9B1B0111609}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1197,7 +1250,7 @@
           <xdr:cNvPr id="21" name="テキスト ボックス 20">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77AF68D4-F358-40D9-895B-BFD595DD4FA3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{77AF68D4-F358-40D9-895B-BFD595DD4FA3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1267,7 +1320,7 @@
         <xdr:cNvPr id="22" name="グループ化 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1243C47E-EC5A-4079-A50A-0FB3F2DF9AF2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1243C47E-EC5A-4079-A50A-0FB3F2DF9AF2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1275,8 +1328,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6057900" y="9906005"/>
-          <a:ext cx="1460913" cy="436018"/>
+          <a:off x="6861175" y="9391655"/>
+          <a:ext cx="1670463" cy="436018"/>
           <a:chOff x="7324725" y="9048750"/>
           <a:chExt cx="1460913" cy="605552"/>
         </a:xfrm>
@@ -1293,7 +1346,7 @@
           <xdr:cNvPr id="23" name="二等辺三角形 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CA828BC-D6DB-4F28-8BE0-27A1608578C3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7CA828BC-D6DB-4F28-8BE0-27A1608578C3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1338,7 +1391,7 @@
           <xdr:cNvPr id="24" name="テキスト ボックス 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84A76F37-BCBE-4260-8069-04FBB43B3309}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84A76F37-BCBE-4260-8069-04FBB43B3309}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1408,7 +1461,7 @@
         <xdr:cNvPr id="25" name="グループ化 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C594A8-C5D6-408E-8363-55521646362C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B9C594A8-C5D6-408E-8363-55521646362C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,8 +1469,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6953250" y="10591805"/>
-          <a:ext cx="734047" cy="436018"/>
+          <a:off x="7896225" y="10067930"/>
+          <a:ext cx="803897" cy="436018"/>
           <a:chOff x="7724775" y="9048750"/>
           <a:chExt cx="734047" cy="605552"/>
         </a:xfrm>
@@ -1434,7 +1487,7 @@
           <xdr:cNvPr id="26" name="二等辺三角形 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A53C0650-3662-482B-BB6F-79910C21E071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A53C0650-3662-482B-BB6F-79910C21E071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1479,7 +1532,7 @@
           <xdr:cNvPr id="27" name="テキスト ボックス 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBF39D9C-A96E-40ED-9592-B25A8E56A41B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DBF39D9C-A96E-40ED-9592-B25A8E56A41B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1549,7 +1602,7 @@
         <xdr:cNvPr id="29" name="グループ化 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{188F4B6C-8177-4D28-A5EB-5A6576CA2E07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{188F4B6C-8177-4D28-A5EB-5A6576CA2E07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1557,8 +1610,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="257175" y="12706350"/>
-          <a:ext cx="7981950" cy="266700"/>
+          <a:off x="292100" y="12153900"/>
+          <a:ext cx="9064625" cy="241300"/>
           <a:chOff x="247650" y="12868275"/>
           <a:chExt cx="7981950" cy="266700"/>
         </a:xfrm>
@@ -1568,7 +1621,7 @@
           <xdr:cNvPr id="5" name="直線矢印コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946F05D2-8024-47CB-BF33-8766A7524144}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{946F05D2-8024-47CB-BF33-8766A7524144}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1607,7 +1660,7 @@
           <xdr:cNvPr id="28" name="テキスト ボックス 27">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB4A3B7-9E13-477B-BECE-DB07E2A519C7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1DB4A3B7-9E13-477B-BECE-DB07E2A519C7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1677,7 +1730,7 @@
         <xdr:cNvPr id="30" name="グループ化 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73E70C19-12F6-4A43-A08E-B3AE0C9A74CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73E70C19-12F6-4A43-A08E-B3AE0C9A74CF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1685,8 +1738,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8239125" y="13258800"/>
-          <a:ext cx="7715250" cy="266700"/>
+          <a:off x="9356725" y="12668250"/>
+          <a:ext cx="8763000" cy="254000"/>
           <a:chOff x="247650" y="12868275"/>
           <a:chExt cx="7981950" cy="266700"/>
         </a:xfrm>
@@ -1696,7 +1749,7 @@
           <xdr:cNvPr id="31" name="直線矢印コネクタ 30">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9040DBEF-EBA2-43BE-AFCA-33F3CABC3161}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9040DBEF-EBA2-43BE-AFCA-33F3CABC3161}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1735,7 +1788,7 @@
           <xdr:cNvPr id="32" name="テキスト ボックス 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE60841B-8509-4415-ACCA-BF25C500ECBD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FE60841B-8509-4415-ACCA-BF25C500ECBD}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1833,7 +1886,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1885,7 +1938,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2079,7 +2132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2089,11 +2142,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BJ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BC49" sqref="BC49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
@@ -2230,73 +2283,73 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:62" ht="15.75" thickBot="1"/>
+    <row r="36" spans="2:62" ht="15" thickBot="1"/>
     <row r="37" spans="2:62">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
-      <c r="AA37" s="9"/>
-      <c r="AB37" s="9"/>
-      <c r="AC37" s="9"/>
-      <c r="AD37" s="9"/>
-      <c r="AE37" s="9"/>
-      <c r="AF37" s="10"/>
-      <c r="AG37" s="9" t="s">
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+      <c r="T37" s="46"/>
+      <c r="U37" s="46"/>
+      <c r="V37" s="46"/>
+      <c r="W37" s="46"/>
+      <c r="X37" s="46"/>
+      <c r="Y37" s="46"/>
+      <c r="Z37" s="46"/>
+      <c r="AA37" s="46"/>
+      <c r="AB37" s="46"/>
+      <c r="AC37" s="46"/>
+      <c r="AD37" s="46"/>
+      <c r="AE37" s="46"/>
+      <c r="AF37" s="47"/>
+      <c r="AG37" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AH37" s="9"/>
-      <c r="AI37" s="9"/>
-      <c r="AJ37" s="9"/>
-      <c r="AK37" s="9"/>
-      <c r="AL37" s="9"/>
-      <c r="AM37" s="9"/>
-      <c r="AN37" s="9"/>
-      <c r="AO37" s="9"/>
-      <c r="AP37" s="9"/>
-      <c r="AQ37" s="9"/>
-      <c r="AR37" s="9"/>
-      <c r="AS37" s="9"/>
-      <c r="AT37" s="9"/>
-      <c r="AU37" s="9"/>
-      <c r="AV37" s="9"/>
-      <c r="AW37" s="9"/>
-      <c r="AX37" s="9"/>
-      <c r="AY37" s="9"/>
-      <c r="AZ37" s="9"/>
-      <c r="BA37" s="9"/>
-      <c r="BB37" s="9"/>
-      <c r="BC37" s="9"/>
-      <c r="BD37" s="9"/>
-      <c r="BE37" s="9"/>
-      <c r="BF37" s="9"/>
-      <c r="BG37" s="9"/>
-      <c r="BH37" s="9"/>
-      <c r="BI37" s="9"/>
-      <c r="BJ37" s="10"/>
+      <c r="AH37" s="46"/>
+      <c r="AI37" s="46"/>
+      <c r="AJ37" s="46"/>
+      <c r="AK37" s="46"/>
+      <c r="AL37" s="46"/>
+      <c r="AM37" s="46"/>
+      <c r="AN37" s="46"/>
+      <c r="AO37" s="46"/>
+      <c r="AP37" s="46"/>
+      <c r="AQ37" s="46"/>
+      <c r="AR37" s="46"/>
+      <c r="AS37" s="46"/>
+      <c r="AT37" s="46"/>
+      <c r="AU37" s="46"/>
+      <c r="AV37" s="46"/>
+      <c r="AW37" s="46"/>
+      <c r="AX37" s="46"/>
+      <c r="AY37" s="46"/>
+      <c r="AZ37" s="46"/>
+      <c r="BA37" s="46"/>
+      <c r="BB37" s="46"/>
+      <c r="BC37" s="46"/>
+      <c r="BD37" s="46"/>
+      <c r="BE37" s="46"/>
+      <c r="BF37" s="46"/>
+      <c r="BG37" s="46"/>
+      <c r="BH37" s="46"/>
+      <c r="BI37" s="46"/>
+      <c r="BJ37" s="47"/>
     </row>
     <row r="38" spans="2:62">
       <c r="B38" s="5">
@@ -2392,7 +2445,7 @@
       <c r="AF38" s="6">
         <v>1</v>
       </c>
-      <c r="AG38" s="15">
+      <c r="AG38" s="12">
         <v>1</v>
       </c>
       <c r="AH38" s="3">
@@ -2577,7 +2630,7 @@
       <c r="AF39" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AG39" s="15" t="s">
+      <c r="AG39" s="12" t="s">
         <v>29</v>
       </c>
       <c r="AH39" s="3" t="s">
@@ -2669,445 +2722,445 @@
       </c>
     </row>
     <row r="40" spans="2:62" ht="57.75" customHeight="1">
-      <c r="B40" s="26"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="13"/>
-      <c r="S40" s="13"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="17"/>
-      <c r="V40" s="12"/>
-      <c r="W40" s="12"/>
-      <c r="X40" s="12"/>
-      <c r="Y40" s="12"/>
-      <c r="Z40" s="12"/>
-      <c r="AA40" s="19"/>
-      <c r="AB40" s="20"/>
-      <c r="AC40" s="21"/>
-      <c r="AD40" s="21"/>
-      <c r="AE40" s="21"/>
-      <c r="AF40" s="46"/>
-      <c r="AG40" s="44"/>
-      <c r="AH40" s="22"/>
-      <c r="AI40" s="23"/>
-      <c r="AJ40" s="24"/>
-      <c r="AK40" s="24"/>
-      <c r="AL40" s="24"/>
-      <c r="AM40" s="24"/>
-      <c r="AN40" s="24"/>
-      <c r="AO40" s="25"/>
-      <c r="AP40" s="18"/>
-      <c r="AQ40" s="13"/>
-      <c r="AR40" s="13"/>
-      <c r="AS40" s="13"/>
-      <c r="AT40" s="13"/>
-      <c r="AU40" s="13"/>
-      <c r="AV40" s="14"/>
-      <c r="AW40" s="23"/>
-      <c r="AX40" s="24"/>
-      <c r="AY40" s="24"/>
-      <c r="AZ40" s="24"/>
-      <c r="BA40" s="24"/>
-      <c r="BB40" s="24"/>
-      <c r="BC40" s="25"/>
-      <c r="BD40" s="18"/>
-      <c r="BE40" s="13"/>
-      <c r="BF40" s="13"/>
-      <c r="BG40" s="13"/>
-      <c r="BH40" s="13"/>
-      <c r="BI40" s="13"/>
-      <c r="BJ40" s="27"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="9"/>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="9"/>
+      <c r="Z40" s="9"/>
+      <c r="AA40" s="16"/>
+      <c r="AB40" s="17"/>
+      <c r="AC40" s="18"/>
+      <c r="AD40" s="18"/>
+      <c r="AE40" s="18"/>
+      <c r="AF40" s="43"/>
+      <c r="AG40" s="41"/>
+      <c r="AH40" s="19"/>
+      <c r="AI40" s="20"/>
+      <c r="AJ40" s="21"/>
+      <c r="AK40" s="21"/>
+      <c r="AL40" s="21"/>
+      <c r="AM40" s="21"/>
+      <c r="AN40" s="21"/>
+      <c r="AO40" s="22"/>
+      <c r="AP40" s="15"/>
+      <c r="AQ40" s="10"/>
+      <c r="AR40" s="10"/>
+      <c r="AS40" s="10"/>
+      <c r="AT40" s="10"/>
+      <c r="AU40" s="10"/>
+      <c r="AV40" s="11"/>
+      <c r="AW40" s="20"/>
+      <c r="AX40" s="21"/>
+      <c r="AY40" s="21"/>
+      <c r="AZ40" s="21"/>
+      <c r="BA40" s="21"/>
+      <c r="BB40" s="21"/>
+      <c r="BC40" s="22"/>
+      <c r="BD40" s="15"/>
+      <c r="BE40" s="10"/>
+      <c r="BF40" s="10"/>
+      <c r="BG40" s="10"/>
+      <c r="BH40" s="10"/>
+      <c r="BI40" s="10"/>
+      <c r="BJ40" s="24"/>
     </row>
     <row r="41" spans="2:62" ht="57.75" customHeight="1">
-      <c r="B41" s="26"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="17"/>
-      <c r="V41" s="12"/>
-      <c r="W41" s="12"/>
-      <c r="X41" s="12"/>
-      <c r="Y41" s="12"/>
-      <c r="Z41" s="12"/>
-      <c r="AA41" s="19"/>
-      <c r="AB41" s="20"/>
-      <c r="AC41" s="21"/>
-      <c r="AD41" s="21"/>
-      <c r="AE41" s="21"/>
-      <c r="AF41" s="46"/>
-      <c r="AG41" s="44"/>
-      <c r="AH41" s="22"/>
-      <c r="AI41" s="23"/>
-      <c r="AJ41" s="24"/>
-      <c r="AK41" s="24"/>
-      <c r="AL41" s="24"/>
-      <c r="AM41" s="24"/>
-      <c r="AN41" s="24"/>
-      <c r="AO41" s="25"/>
-      <c r="AP41" s="18"/>
-      <c r="AQ41" s="13"/>
-      <c r="AR41" s="13"/>
-      <c r="AS41" s="13"/>
-      <c r="AT41" s="13"/>
-      <c r="AU41" s="13"/>
-      <c r="AV41" s="14"/>
-      <c r="AW41" s="23"/>
-      <c r="AX41" s="24"/>
-      <c r="AY41" s="24"/>
-      <c r="AZ41" s="24"/>
-      <c r="BA41" s="24"/>
-      <c r="BB41" s="24"/>
-      <c r="BC41" s="25"/>
-      <c r="BD41" s="18"/>
-      <c r="BE41" s="13"/>
-      <c r="BF41" s="13"/>
-      <c r="BG41" s="13"/>
-      <c r="BH41" s="13"/>
-      <c r="BI41" s="13"/>
-      <c r="BJ41" s="27"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="9"/>
+      <c r="W41" s="9"/>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="9"/>
+      <c r="Z41" s="9"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="17"/>
+      <c r="AC41" s="18"/>
+      <c r="AD41" s="18"/>
+      <c r="AE41" s="18"/>
+      <c r="AF41" s="43"/>
+      <c r="AG41" s="41"/>
+      <c r="AH41" s="19"/>
+      <c r="AI41" s="20"/>
+      <c r="AJ41" s="21"/>
+      <c r="AK41" s="21"/>
+      <c r="AL41" s="21"/>
+      <c r="AM41" s="21"/>
+      <c r="AN41" s="21"/>
+      <c r="AO41" s="22"/>
+      <c r="AP41" s="15"/>
+      <c r="AQ41" s="10"/>
+      <c r="AR41" s="10"/>
+      <c r="AS41" s="10"/>
+      <c r="AT41" s="10"/>
+      <c r="AU41" s="10"/>
+      <c r="AV41" s="11"/>
+      <c r="AW41" s="20"/>
+      <c r="AX41" s="21"/>
+      <c r="AY41" s="21"/>
+      <c r="AZ41" s="21"/>
+      <c r="BA41" s="21"/>
+      <c r="BB41" s="21"/>
+      <c r="BC41" s="22"/>
+      <c r="BD41" s="15"/>
+      <c r="BE41" s="10"/>
+      <c r="BF41" s="10"/>
+      <c r="BG41" s="10"/>
+      <c r="BH41" s="10"/>
+      <c r="BI41" s="10"/>
+      <c r="BJ41" s="24"/>
     </row>
     <row r="42" spans="2:62" ht="57.75" customHeight="1">
-      <c r="B42" s="26"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="13"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="17"/>
-      <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
-      <c r="X42" s="12"/>
-      <c r="Y42" s="12"/>
-      <c r="Z42" s="12"/>
-      <c r="AA42" s="19"/>
-      <c r="AB42" s="20"/>
-      <c r="AC42" s="21"/>
-      <c r="AD42" s="21"/>
-      <c r="AE42" s="21"/>
-      <c r="AF42" s="46"/>
-      <c r="AG42" s="44"/>
-      <c r="AH42" s="22"/>
-      <c r="AI42" s="23"/>
-      <c r="AJ42" s="24"/>
-      <c r="AK42" s="24"/>
-      <c r="AL42" s="24"/>
-      <c r="AM42" s="24"/>
-      <c r="AN42" s="24"/>
-      <c r="AO42" s="25"/>
-      <c r="AP42" s="18"/>
-      <c r="AQ42" s="13"/>
-      <c r="AR42" s="13"/>
-      <c r="AS42" s="13"/>
-      <c r="AT42" s="13"/>
-      <c r="AU42" s="13"/>
-      <c r="AV42" s="14"/>
-      <c r="AW42" s="23"/>
-      <c r="AX42" s="24"/>
-      <c r="AY42" s="24"/>
-      <c r="AZ42" s="24"/>
-      <c r="BA42" s="24"/>
-      <c r="BB42" s="24"/>
-      <c r="BC42" s="25"/>
-      <c r="BD42" s="18"/>
-      <c r="BE42" s="13"/>
-      <c r="BF42" s="13"/>
-      <c r="BG42" s="13"/>
-      <c r="BH42" s="13"/>
-      <c r="BI42" s="13"/>
-      <c r="BJ42" s="27"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="9"/>
+      <c r="W42" s="9"/>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="9"/>
+      <c r="Z42" s="9"/>
+      <c r="AA42" s="16"/>
+      <c r="AB42" s="17"/>
+      <c r="AC42" s="18"/>
+      <c r="AD42" s="18"/>
+      <c r="AE42" s="18"/>
+      <c r="AF42" s="43"/>
+      <c r="AG42" s="41"/>
+      <c r="AH42" s="19"/>
+      <c r="AI42" s="20"/>
+      <c r="AJ42" s="21"/>
+      <c r="AK42" s="21"/>
+      <c r="AL42" s="21"/>
+      <c r="AM42" s="21"/>
+      <c r="AN42" s="21"/>
+      <c r="AO42" s="22"/>
+      <c r="AP42" s="15"/>
+      <c r="AQ42" s="10"/>
+      <c r="AR42" s="10"/>
+      <c r="AS42" s="10"/>
+      <c r="AT42" s="10"/>
+      <c r="AU42" s="10"/>
+      <c r="AV42" s="11"/>
+      <c r="AW42" s="20"/>
+      <c r="AX42" s="21"/>
+      <c r="AY42" s="21"/>
+      <c r="AZ42" s="21"/>
+      <c r="BA42" s="21"/>
+      <c r="BB42" s="21"/>
+      <c r="BC42" s="22"/>
+      <c r="BD42" s="15"/>
+      <c r="BE42" s="10"/>
+      <c r="BF42" s="10"/>
+      <c r="BG42" s="10"/>
+      <c r="BH42" s="10"/>
+      <c r="BI42" s="10"/>
+      <c r="BJ42" s="24"/>
     </row>
     <row r="43" spans="2:62" ht="57.75" customHeight="1">
-      <c r="B43" s="26"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="13"/>
-      <c r="S43" s="13"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="17"/>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
-      <c r="AA43" s="19"/>
-      <c r="AB43" s="20"/>
-      <c r="AC43" s="21"/>
-      <c r="AD43" s="21"/>
-      <c r="AE43" s="21"/>
-      <c r="AF43" s="46"/>
-      <c r="AG43" s="44"/>
-      <c r="AH43" s="22"/>
-      <c r="AI43" s="23"/>
-      <c r="AJ43" s="24"/>
-      <c r="AK43" s="24"/>
-      <c r="AL43" s="24"/>
-      <c r="AM43" s="24"/>
-      <c r="AN43" s="24"/>
-      <c r="AO43" s="25"/>
-      <c r="AP43" s="18"/>
-      <c r="AQ43" s="13"/>
-      <c r="AR43" s="13"/>
-      <c r="AS43" s="13"/>
-      <c r="AT43" s="13"/>
-      <c r="AU43" s="13"/>
-      <c r="AV43" s="14"/>
-      <c r="AW43" s="23"/>
-      <c r="AX43" s="24"/>
-      <c r="AY43" s="24"/>
-      <c r="AZ43" s="24"/>
-      <c r="BA43" s="24"/>
-      <c r="BB43" s="24"/>
-      <c r="BC43" s="25"/>
-      <c r="BD43" s="18"/>
-      <c r="BE43" s="13"/>
-      <c r="BF43" s="13"/>
-      <c r="BG43" s="13"/>
-      <c r="BH43" s="13"/>
-      <c r="BI43" s="13"/>
-      <c r="BJ43" s="27"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="9"/>
+      <c r="Z43" s="9"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="17"/>
+      <c r="AC43" s="18"/>
+      <c r="AD43" s="18"/>
+      <c r="AE43" s="18"/>
+      <c r="AF43" s="43"/>
+      <c r="AG43" s="41"/>
+      <c r="AH43" s="19"/>
+      <c r="AI43" s="20"/>
+      <c r="AJ43" s="21"/>
+      <c r="AK43" s="21"/>
+      <c r="AL43" s="21"/>
+      <c r="AM43" s="21"/>
+      <c r="AN43" s="21"/>
+      <c r="AO43" s="22"/>
+      <c r="AP43" s="15"/>
+      <c r="AQ43" s="10"/>
+      <c r="AR43" s="10"/>
+      <c r="AS43" s="10"/>
+      <c r="AT43" s="10"/>
+      <c r="AU43" s="10"/>
+      <c r="AV43" s="11"/>
+      <c r="AW43" s="20"/>
+      <c r="AX43" s="21"/>
+      <c r="AY43" s="21"/>
+      <c r="AZ43" s="21"/>
+      <c r="BA43" s="21"/>
+      <c r="BB43" s="21"/>
+      <c r="BC43" s="22"/>
+      <c r="BD43" s="15"/>
+      <c r="BE43" s="10"/>
+      <c r="BF43" s="10"/>
+      <c r="BG43" s="10"/>
+      <c r="BH43" s="10"/>
+      <c r="BI43" s="10"/>
+      <c r="BJ43" s="24"/>
     </row>
     <row r="44" spans="2:62" ht="57.75" customHeight="1">
-      <c r="B44" s="26"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="13"/>
-      <c r="S44" s="13"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="17"/>
-      <c r="V44" s="12"/>
-      <c r="W44" s="12"/>
-      <c r="X44" s="12"/>
-      <c r="Y44" s="12"/>
-      <c r="Z44" s="12"/>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="20"/>
-      <c r="AC44" s="21"/>
-      <c r="AD44" s="21"/>
-      <c r="AE44" s="21"/>
-      <c r="AF44" s="46"/>
-      <c r="AG44" s="44"/>
-      <c r="AH44" s="22"/>
-      <c r="AI44" s="23"/>
-      <c r="AJ44" s="24"/>
-      <c r="AK44" s="24"/>
-      <c r="AL44" s="24"/>
-      <c r="AM44" s="24"/>
-      <c r="AN44" s="24"/>
-      <c r="AO44" s="25"/>
-      <c r="AP44" s="18"/>
-      <c r="AQ44" s="13"/>
-      <c r="AR44" s="13"/>
-      <c r="AS44" s="13"/>
-      <c r="AT44" s="13"/>
-      <c r="AU44" s="13"/>
-      <c r="AV44" s="14"/>
-      <c r="AW44" s="23"/>
-      <c r="AX44" s="24"/>
-      <c r="AY44" s="24"/>
-      <c r="AZ44" s="24"/>
-      <c r="BA44" s="24"/>
-      <c r="BB44" s="24"/>
-      <c r="BC44" s="25"/>
-      <c r="BD44" s="18"/>
-      <c r="BE44" s="13"/>
-      <c r="BF44" s="13"/>
-      <c r="BG44" s="13"/>
-      <c r="BH44" s="13"/>
-      <c r="BI44" s="13"/>
-      <c r="BJ44" s="27"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="9"/>
+      <c r="W44" s="9"/>
+      <c r="X44" s="9"/>
+      <c r="Y44" s="9"/>
+      <c r="Z44" s="9"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="17"/>
+      <c r="AC44" s="18"/>
+      <c r="AD44" s="18"/>
+      <c r="AE44" s="18"/>
+      <c r="AF44" s="43"/>
+      <c r="AG44" s="41"/>
+      <c r="AH44" s="19"/>
+      <c r="AI44" s="20"/>
+      <c r="AJ44" s="21"/>
+      <c r="AK44" s="21"/>
+      <c r="AL44" s="21"/>
+      <c r="AM44" s="21"/>
+      <c r="AN44" s="21"/>
+      <c r="AO44" s="22"/>
+      <c r="AP44" s="15"/>
+      <c r="AQ44" s="10"/>
+      <c r="AR44" s="10"/>
+      <c r="AS44" s="10"/>
+      <c r="AT44" s="10"/>
+      <c r="AU44" s="10"/>
+      <c r="AV44" s="11"/>
+      <c r="AW44" s="20"/>
+      <c r="AX44" s="21"/>
+      <c r="AY44" s="21"/>
+      <c r="AZ44" s="21"/>
+      <c r="BA44" s="21"/>
+      <c r="BB44" s="21"/>
+      <c r="BC44" s="22"/>
+      <c r="BD44" s="15"/>
+      <c r="BE44" s="10"/>
+      <c r="BF44" s="10"/>
+      <c r="BG44" s="10"/>
+      <c r="BH44" s="10"/>
+      <c r="BI44" s="10"/>
+      <c r="BJ44" s="24"/>
     </row>
     <row r="45" spans="2:62" ht="57.75" customHeight="1">
-      <c r="B45" s="26"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="13"/>
-      <c r="S45" s="13"/>
-      <c r="T45" s="14"/>
-      <c r="U45" s="17"/>
-      <c r="V45" s="12"/>
-      <c r="W45" s="12"/>
-      <c r="X45" s="12"/>
-      <c r="Y45" s="12"/>
-      <c r="Z45" s="12"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="20"/>
-      <c r="AC45" s="21"/>
-      <c r="AD45" s="21"/>
-      <c r="AE45" s="21"/>
-      <c r="AF45" s="46"/>
-      <c r="AG45" s="44"/>
-      <c r="AH45" s="22"/>
-      <c r="AI45" s="23"/>
-      <c r="AJ45" s="24"/>
-      <c r="AK45" s="24"/>
-      <c r="AL45" s="24"/>
-      <c r="AM45" s="24"/>
-      <c r="AN45" s="24"/>
-      <c r="AO45" s="25"/>
-      <c r="AP45" s="18"/>
-      <c r="AQ45" s="13"/>
-      <c r="AR45" s="13"/>
-      <c r="AS45" s="13"/>
-      <c r="AT45" s="13"/>
-      <c r="AU45" s="13"/>
-      <c r="AV45" s="14"/>
-      <c r="AW45" s="23"/>
-      <c r="AX45" s="24"/>
-      <c r="AY45" s="24"/>
-      <c r="AZ45" s="24"/>
-      <c r="BA45" s="24"/>
-      <c r="BB45" s="24"/>
-      <c r="BC45" s="25"/>
-      <c r="BD45" s="18"/>
-      <c r="BE45" s="13"/>
-      <c r="BF45" s="13"/>
-      <c r="BG45" s="13"/>
-      <c r="BH45" s="13"/>
-      <c r="BI45" s="13"/>
-      <c r="BJ45" s="27"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="22"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="9"/>
+      <c r="W45" s="9"/>
+      <c r="X45" s="9"/>
+      <c r="Y45" s="9"/>
+      <c r="Z45" s="9"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="17"/>
+      <c r="AC45" s="18"/>
+      <c r="AD45" s="18"/>
+      <c r="AE45" s="18"/>
+      <c r="AF45" s="43"/>
+      <c r="AG45" s="41"/>
+      <c r="AH45" s="19"/>
+      <c r="AI45" s="20"/>
+      <c r="AJ45" s="21"/>
+      <c r="AK45" s="21"/>
+      <c r="AL45" s="21"/>
+      <c r="AM45" s="21"/>
+      <c r="AN45" s="21"/>
+      <c r="AO45" s="22"/>
+      <c r="AP45" s="15"/>
+      <c r="AQ45" s="10"/>
+      <c r="AR45" s="10"/>
+      <c r="AS45" s="10"/>
+      <c r="AT45" s="10"/>
+      <c r="AU45" s="10"/>
+      <c r="AV45" s="11"/>
+      <c r="AW45" s="20"/>
+      <c r="AX45" s="21"/>
+      <c r="AY45" s="21"/>
+      <c r="AZ45" s="21"/>
+      <c r="BA45" s="21"/>
+      <c r="BB45" s="21"/>
+      <c r="BC45" s="22"/>
+      <c r="BD45" s="15"/>
+      <c r="BE45" s="10"/>
+      <c r="BF45" s="10"/>
+      <c r="BG45" s="10"/>
+      <c r="BH45" s="10"/>
+      <c r="BI45" s="10"/>
+      <c r="BJ45" s="24"/>
     </row>
     <row r="46" spans="2:62" ht="57.75" customHeight="1" thickBot="1">
-      <c r="B46" s="28"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="33"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="35"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="35"/>
-      <c r="R46" s="35"/>
-      <c r="S46" s="35"/>
-      <c r="T46" s="36"/>
-      <c r="U46" s="37"/>
-      <c r="V46" s="38"/>
-      <c r="W46" s="38"/>
-      <c r="X46" s="38"/>
-      <c r="Y46" s="38"/>
-      <c r="Z46" s="38"/>
-      <c r="AA46" s="39"/>
-      <c r="AB46" s="40"/>
-      <c r="AC46" s="41"/>
-      <c r="AD46" s="41"/>
-      <c r="AE46" s="41"/>
-      <c r="AF46" s="47"/>
-      <c r="AG46" s="45"/>
-      <c r="AH46" s="42"/>
-      <c r="AI46" s="31"/>
-      <c r="AJ46" s="32"/>
-      <c r="AK46" s="32"/>
-      <c r="AL46" s="32"/>
-      <c r="AM46" s="32"/>
-      <c r="AN46" s="32"/>
-      <c r="AO46" s="33"/>
-      <c r="AP46" s="34"/>
-      <c r="AQ46" s="35"/>
-      <c r="AR46" s="35"/>
-      <c r="AS46" s="35"/>
-      <c r="AT46" s="35"/>
-      <c r="AU46" s="35"/>
-      <c r="AV46" s="36"/>
-      <c r="AW46" s="31"/>
-      <c r="AX46" s="32"/>
-      <c r="AY46" s="32"/>
-      <c r="AZ46" s="32"/>
-      <c r="BA46" s="32"/>
-      <c r="BB46" s="32"/>
-      <c r="BC46" s="33"/>
-      <c r="BD46" s="34"/>
-      <c r="BE46" s="35"/>
-      <c r="BF46" s="35"/>
-      <c r="BG46" s="35"/>
-      <c r="BH46" s="35"/>
-      <c r="BI46" s="35"/>
-      <c r="BJ46" s="43"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="33"/>
+      <c r="U46" s="34"/>
+      <c r="V46" s="35"/>
+      <c r="W46" s="35"/>
+      <c r="X46" s="35"/>
+      <c r="Y46" s="35"/>
+      <c r="Z46" s="35"/>
+      <c r="AA46" s="36"/>
+      <c r="AB46" s="37"/>
+      <c r="AC46" s="38"/>
+      <c r="AD46" s="38"/>
+      <c r="AE46" s="38"/>
+      <c r="AF46" s="44"/>
+      <c r="AG46" s="42"/>
+      <c r="AH46" s="39"/>
+      <c r="AI46" s="28"/>
+      <c r="AJ46" s="29"/>
+      <c r="AK46" s="29"/>
+      <c r="AL46" s="29"/>
+      <c r="AM46" s="29"/>
+      <c r="AN46" s="29"/>
+      <c r="AO46" s="30"/>
+      <c r="AP46" s="31"/>
+      <c r="AQ46" s="32"/>
+      <c r="AR46" s="32"/>
+      <c r="AS46" s="32"/>
+      <c r="AT46" s="32"/>
+      <c r="AU46" s="32"/>
+      <c r="AV46" s="33"/>
+      <c r="AW46" s="28"/>
+      <c r="AX46" s="29"/>
+      <c r="AY46" s="29"/>
+      <c r="AZ46" s="29"/>
+      <c r="BA46" s="29"/>
+      <c r="BB46" s="29"/>
+      <c r="BC46" s="30"/>
+      <c r="BD46" s="31"/>
+      <c r="BE46" s="32"/>
+      <c r="BF46" s="32"/>
+      <c r="BG46" s="32"/>
+      <c r="BH46" s="32"/>
+      <c r="BI46" s="32"/>
+      <c r="BJ46" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3115,7 +3168,122 @@
     <mergeCell ref="AG37:BJ37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>